<commit_message>
update sebelum ganti perangkat
</commit_message>
<xml_diff>
--- a/upload/format.xlsx
+++ b/upload/format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\galih_ta\rodenstock\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34AED4D5-B105-493A-B40C-71DC4B787B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B8704F-232F-4030-9124-2EB20F29A928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{949211B7-5055-4FAA-99FF-7F8A3D203605}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>nim</t>
   </si>
@@ -57,9 +57,6 @@
     <t>nama_sertifikat</t>
   </si>
   <si>
-    <t>jenis_sertifikkat</t>
-  </si>
-  <si>
     <t>nama_organisasi</t>
   </si>
   <si>
@@ -148,6 +145,18 @@
   </si>
   <si>
     <t>Andre</t>
+  </si>
+  <si>
+    <t>tahun_akademik</t>
+  </si>
+  <si>
+    <t>jenis_sertifikat</t>
+  </si>
+  <si>
+    <t>prodi</t>
+  </si>
+  <si>
+    <t>04</t>
   </si>
 </sst>
 </file>
@@ -197,9 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31DCA58-7128-48E7-BA4F-5451A95D67DB}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,18 +536,18 @@
     <col min="4" max="4" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.109375" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>37</v>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -551,36 +562,42 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>19090074</v>
+        <v>19090001</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>50000000</v>
@@ -588,11 +605,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
+      <c r="G2">
+        <v>2019</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
@@ -604,32 +621,38 @@
         <v>24</v>
       </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>19090001</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>19090002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>19090074</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>19090076</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
       </c>
       <c r="E4">
         <v>50000002</v>
@@ -637,59 +660,65 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
+      <c r="G4">
+        <v>2019</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
       </c>
       <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19090002</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>19090002</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>19090003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>19090076</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>19090076</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>19090079</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
       </c>
       <c r="E7">
         <v>50000005</v>
@@ -697,69 +726,75 @@
       <c r="F7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>2019</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>19090003</v>
+      </c>
+      <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>19090003</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" t="s">
         <v>14</v>
       </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>19090079</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="M9" t="s">
         <v>35</v>
       </c>
-      <c r="L8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>19090079</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" t="s">
-        <v>22</v>
+      <c r="N9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>